<commit_message>
feat: 75 exercise heap
</commit_message>
<xml_diff>
--- a/exercise/leetcode-75.xlsx
+++ b/exercise/leetcode-75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\github\datastructure-js\exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18AB8EC-0B67-408C-811D-02B91A58E48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1333207-4FC5-4303-AAF1-0C86F1C743C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
   <si>
     <t>Topics</t>
   </si>
@@ -192,6 +192,49 @@
   <si>
     <t>1. Convert from matrix to simple graphs
 2. DFS the graphs and find the provinces</t>
+  </si>
+  <si>
+    <t>Reorder Routes to Make All Paths Lead to the City Zero</t>
+  </si>
+  <si>
+    <t>1. Save 2 data (graphs and neighbors)
+2. Perform DFS to neighbors
+3. Check if other unvisited neighbors need to be reroute</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=m17yOR5_PpI&amp;ab_channel=NeetCode</t>
+  </si>
+  <si>
+    <t>Evaluate Division</t>
+  </si>
+  <si>
+    <t>1. Save graph data into nodes (value, variable, undir)
+2. DFS the graphs and calculate the math</t>
+  </si>
+  <si>
+    <t>Nearest Exit from Entrance in Maze</t>
+  </si>
+  <si>
+    <t>1. Define Queue and Visited
+2. Do BFS Iteration</t>
+  </si>
+  <si>
+    <t>Rotting Oranges</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?time_continue=164&amp;v=h3GivLJBUTk&amp;embeds_referring_euri=https%3A%2F%2Fleetcode.com%2F&amp;source_ve_path=MTM5MTE3LDEzOTExNywxMzkxMTcsMTM5MTE3LDEzOTExNywyODY2Ng</t>
+  </si>
+  <si>
+    <t>Kth Largest Element in an Array</t>
+  </si>
+  <si>
+    <t>Heap</t>
+  </si>
+  <si>
+    <t>1. Make array with k length (fill it with value of nums[:k])
+2. Heapify the array (min heap)
+3. Loop the remaining nums (nums[k:])
+4. Validate if num greater than peek heap: pop heap and push the greater num</t>
   </si>
 </sst>
 </file>
@@ -242,7 +285,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -261,9 +304,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -272,6 +312,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -389,13 +435,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D5E052F-1221-46EF-A2F3-764ECE85EE2A}" name="Table1" displayName="Table1" ref="B2:F18" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D5E052F-1221-46EF-A2F3-764ECE85EE2A}" name="Table1" displayName="Table1" ref="B2:F23" totalsRowShown="0" headerRowDxfId="5">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{5AEF462A-1184-492E-9180-EA19F478A699}" name="Topics" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{8198827E-B578-435A-83F3-5AA3089541C6}" name="Number" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{54B5D8A8-152C-4E6A-8092-2FFA8DC31C0F}" name="Name" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{8198827E-B578-435A-83F3-5AA3089541C6}" name="Number" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{54B5D8A8-152C-4E6A-8092-2FFA8DC31C0F}" name="Name" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{3696614A-538D-4C79-93A8-C7F1C4527E6F}" name="Steps" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{3A773B8E-1F25-4B7A-B6CF-1F4709BD30F4}" name="Remarks" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{3A773B8E-1F25-4B7A-B6CF-1F4709BD30F4}" name="Remarks" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -664,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F18"/>
+  <dimension ref="B2:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +741,7 @@
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -706,7 +752,7 @@
       <c r="C3" s="5">
         <v>724</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -721,7 +767,7 @@
       <c r="C4" s="6">
         <v>1657</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -736,7 +782,7 @@
       <c r="C5" s="6">
         <v>2352</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -751,7 +797,7 @@
       <c r="C6" s="6">
         <v>2390</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="7" t="s">
@@ -766,13 +812,13 @@
       <c r="C7" s="6">
         <v>394</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="10" t="s">
         <v>17</v>
       </c>
     </row>
@@ -783,13 +829,13 @@
       <c r="C8" s="6">
         <v>649</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -800,7 +846,7 @@
       <c r="C9" s="6">
         <v>328</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -815,7 +861,7 @@
       <c r="C10" s="6">
         <v>206</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>26</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -830,7 +876,7 @@
       <c r="C11" s="6">
         <v>2130</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="7" t="s">
@@ -845,7 +891,7 @@
       <c r="C12" s="6">
         <v>437</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E12" s="7" t="s">
@@ -860,7 +906,7 @@
       <c r="C13" s="6">
         <v>1372</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>33</v>
       </c>
       <c r="E13" s="7" t="s">
@@ -890,7 +936,7 @@
       <c r="C15" s="6">
         <v>199</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>37</v>
       </c>
       <c r="E15" s="7" t="s">
@@ -905,7 +951,7 @@
       <c r="C16" s="6">
         <v>1161</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E16" s="7" t="s">
@@ -920,7 +966,7 @@
       <c r="C17" s="6">
         <v>841</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E17" s="7" t="s">
@@ -935,13 +981,92 @@
       <c r="C18" s="6">
         <v>547</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="8" t="s">
         <v>45</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>46</v>
       </c>
       <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1466</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="6">
+        <v>399</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="6">
+        <v>1926</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="6">
+        <v>994</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="6">
+        <v>215</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -963,11 +1088,18 @@
     <hyperlink ref="D16" r:id="rId16" display="https://leetcode.com/problems/maximum-level-sum-of-a-binary-tree/" xr:uid="{507D57CF-09E1-4325-A4D7-0232882A7C4C}"/>
     <hyperlink ref="D17" r:id="rId17" display="https://leetcode.com/problems/keys-and-rooms/" xr:uid="{5AEFA21A-B1A3-452F-A372-7023F85F9F66}"/>
     <hyperlink ref="D18" r:id="rId18" display="https://leetcode.com/problems/number-of-provinces/" xr:uid="{1678016C-B127-49E2-BCF9-BEBAE7D3C690}"/>
+    <hyperlink ref="D19" r:id="rId19" display="https://leetcode.com/problems/reorder-routes-to-make-all-paths-lead-to-the-city-zero/" xr:uid="{132BAFB6-FDE0-43A3-9486-C2285DCE9F08}"/>
+    <hyperlink ref="F19" r:id="rId20" xr:uid="{3772D2D8-C380-4095-A45C-F8D1ED1B0882}"/>
+    <hyperlink ref="D20" r:id="rId21" display="https://leetcode.com/problems/evaluate-division/" xr:uid="{CA8B2B27-BF6F-4D9B-AE91-1C001D901ED7}"/>
+    <hyperlink ref="D21" r:id="rId22" display="https://leetcode.com/problems/nearest-exit-from-entrance-in-maze/" xr:uid="{A2D4E9CE-43B4-4525-9006-7EF53CA3F000}"/>
+    <hyperlink ref="D22" r:id="rId23" display="https://leetcode.com/problems/rotting-oranges/" xr:uid="{3161E5F4-8AA8-439A-B3C3-42338BEA5ADF}"/>
+    <hyperlink ref="F23" r:id="rId24" xr:uid="{4EFAC4DA-18FF-4D55-97AE-7BFE7D2951DE}"/>
+    <hyperlink ref="D23" r:id="rId25" display="https://leetcode.com/problems/kth-largest-element-in-an-array/" xr:uid="{BA953054-0D00-4F90-8FDB-8B4025C82DB7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId19"/>
+  <drawing r:id="rId26"/>
   <tableParts count="1">
-    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId27"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: finish leetcode 75
</commit_message>
<xml_diff>
--- a/exercise/leetcode-75.xlsx
+++ b/exercise/leetcode-75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK\TSP - CODE\datastructure-js\exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E999DCE-9DBC-4230-93BB-0F2E2317A4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382856B4-DD34-4655-BC8B-BD27592EB3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="91">
   <si>
     <t>Topics</t>
   </si>
@@ -317,6 +317,34 @@
   </si>
   <si>
     <t>Multi-DP</t>
+  </si>
+  <si>
+    <t>Non-overlapping Intervals</t>
+  </si>
+  <si>
+    <t>Intervals</t>
+  </si>
+  <si>
+    <t>1. Sort based on the first num
+2. Create right variable, Iterate over the arr[1:]
+3. Calculate the right variable</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=nONCGxWoUfM&amp;ab_channel=NeetCode</t>
+  </si>
+  <si>
+    <t>Daily Temperatures</t>
+  </si>
+  <si>
+    <t>Monotonic Stacks</t>
+  </si>
+  <si>
+    <t>1. Initiate array and monotonic stack
+2. Iterate the values validate current is more than monotonic stack peek, if yes while loop to remove
+3. Don’t forget every iterate need to append to the stack</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=cTBiBSnjO3c&amp;ab_channel=NeetCode</t>
   </si>
 </sst>
 </file>
@@ -528,7 +556,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D5E052F-1221-46EF-A2F3-764ECE85EE2A}" name="Table1" displayName="Table1" ref="B2:F32" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D5E052F-1221-46EF-A2F3-764ECE85EE2A}" name="Table1" displayName="Table1" ref="B2:F34" totalsRowShown="0" headerRowDxfId="5">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{5AEF462A-1184-492E-9180-EA19F478A699}" name="Topics" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{8198827E-B578-435A-83F3-5AA3089541C6}" name="Number" dataDxfId="3"/>
@@ -803,16 +831,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F32"/>
+  <dimension ref="B2:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="39.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52.28515625" style="2" customWidth="1"/>
@@ -1298,6 +1326,40 @@
       </c>
       <c r="F32" s="9" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B33" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="5">
+        <v>435</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B34" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="5">
+        <v>739</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1338,12 +1400,16 @@
     <hyperlink ref="F31" r:id="rId34" xr:uid="{4B4FB093-4580-480F-92D3-E00FA7A24669}"/>
     <hyperlink ref="F32" r:id="rId35" xr:uid="{EC6DDAEA-A6FA-4D46-BDBD-AE104F06AB3C}"/>
     <hyperlink ref="D32" r:id="rId36" display="https://leetcode.com/problems/unique-paths/" xr:uid="{24D3DDD3-0C52-45BA-94F7-9ADBA810D69A}"/>
+    <hyperlink ref="D33" r:id="rId37" display="https://leetcode.com/problems/non-overlapping-intervals/" xr:uid="{26C640FB-B32A-47F9-AF9F-CAFC17FB0BD0}"/>
+    <hyperlink ref="F33" r:id="rId38" xr:uid="{C6C403CC-C252-4CA1-8E0D-B11A740C1AB8}"/>
+    <hyperlink ref="D34" r:id="rId39" display="https://leetcode.com/problems/daily-temperatures/" xr:uid="{441BC8F9-1FD8-49D8-AFB8-0114CE2DBEE4}"/>
+    <hyperlink ref="F34" r:id="rId40" xr:uid="{1609832C-98A0-45C7-8C74-B7F91F0529B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId37"/>
-  <drawing r:id="rId38"/>
+  <pageSetup orientation="portrait" r:id="rId41"/>
+  <drawing r:id="rId42"/>
   <tableParts count="1">
-    <tablePart r:id="rId39"/>
+    <tablePart r:id="rId43"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>